<commit_message>
code with colour schemes
</commit_message>
<xml_diff>
--- a/BranchInes/Scripts_inesdattatreya/fig_output/LCA_model_fit_table.xlsx
+++ b/BranchInes/Scripts_inesdattatreya/fig_output/LCA_model_fit_table.xlsx
@@ -1,47 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29328"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://tud365-my.sharepoint.com/personal/idattatreya_tudelft_nl/Documents/BEP/R data analysis/BranchInes/Scripts_inesdattatreya/fig_output/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="6" documentId="11_ED6FFDCE8F79A8D366075C52F3E95276F7BADD71" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{AF2A181A-C857-4E04-BBA1-1223EECD8C89}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
-  <si>
-    <t>Classes</t>
-  </si>
-  <si>
-    <t>LogLikelihood</t>
-  </si>
-  <si>
-    <t>AIC</t>
-  </si>
-  <si>
-    <t>BIC</t>
-  </si>
-  <si>
-    <t>Entropy</t>
-  </si>
-</sst>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -85,126 +59,17 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Standaard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="10">
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-  </dxfs>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Office 2007 - 2010">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -242,7 +107,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2007 - 2010">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -276,7 +141,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -311,10 +175,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2007 - 2010">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -487,37 +350,41 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="14.77734375" customWidth="1"/>
-    <col min="2" max="2" width="11.88671875" customWidth="1"/>
-  </cols>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
+    <row r="1" s="1" customFormat="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Classes</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>LogLikelihood</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>AIC</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>BIC</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Entropy</t>
+        </is>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2">
       <c r="A2">
         <v>2</v>
       </c>
@@ -531,71 +398,61 @@
         <v>4042.419232253983</v>
       </c>
       <c r="E2">
-        <v>0.81432645749063504</v>
+        <v>0.814326457490635</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3">
       <c r="A3">
         <v>3</v>
       </c>
       <c r="B3">
-        <v>-1762.8002048079099</v>
+        <v>-1762.80020480791</v>
       </c>
       <c r="C3">
-        <v>3763.6004096158199</v>
+        <v>3763.60040961582</v>
       </c>
       <c r="D3">
-        <v>4123.4421915965268</v>
+        <v>4123.442191596527</v>
       </c>
       <c r="E3">
-        <v>0.90128744657675519</v>
+        <v>0.9012874465767552</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4">
       <c r="A4">
         <v>4</v>
       </c>
       <c r="B4">
-        <v>-1768.5520841785519</v>
+        <v>-1768.552084178552</v>
       </c>
       <c r="C4">
-        <v>3855.1041683571038</v>
+        <v>3855.104168357104</v>
       </c>
       <c r="D4">
-        <v>4335.9011711716621</v>
+        <v>4335.901171171662</v>
       </c>
       <c r="E4">
-        <v>0.90771879897704277</v>
+        <v>0.9077187989770428</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5">
       <c r="A5">
         <v>5</v>
       </c>
       <c r="B5">
-        <v>-1694.3601720260831</v>
+        <v>-1694.360172026083</v>
       </c>
       <c r="C5">
-        <v>3786.7203440521662</v>
+        <v>3786.720344052166</v>
       </c>
       <c r="D5">
-        <v>4388.4725677005754</v>
+        <v>4388.472567700575</v>
       </c>
       <c r="E5">
-        <v>0.92582827856258887</v>
+        <v>0.9258282785625889</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="E2:E5">
-    <cfRule type="top10" dxfId="6" priority="4" percent="1" rank="10"/>
-    <cfRule type="top10" dxfId="5" priority="3" rank="1"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C2:D5">
-    <cfRule type="top10" dxfId="4" priority="2" bottom="1" rank="1"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D2:D5">
-    <cfRule type="top10" dxfId="0" priority="1" percent="1" bottom="1" rank="10"/>
-  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>